<commit_message>
additional datums and detection parts
</commit_message>
<xml_diff>
--- a/ontologies/loinc_obo_assay_template_more_harmonious.xlsx
+++ b/ontologies/loinc_obo_assay_template_more_harmonious.xlsx
@@ -44,7 +44,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-automate the generation of these labels
+MAM todo: automate the generation of these labels
 Assume point-in-time, mass/volume and quantitative? See material processing and output notes.</t>
         </r>
       </text>
@@ -69,7 +69,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-LOINC's "long common name"</t>
+FYI: LOINC's "long common name"</t>
         </r>
       </text>
     </comment>
@@ -142,7 +142,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-MAM todo: add "automated cell counting" and "confirmatory (something?) to TURBO ontology</t>
+MAM done/check: add "automated cell counting" and "confirmatory" processes  to TURBO ontology</t>
         </r>
       </text>
     </comment>
@@ -190,7 +190,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-omit in favor of the evaluant column?</t>
+omitted in favor of the evaluant column</t>
         </r>
       </text>
     </comment>
@@ -215,7 +215,7 @@
           </rPr>
           <t xml:space="preserve">
 Chris used a value specification approach: measurement datum and ( has value specification some scalar value specification (and has_part some mass per unit volume))
-MAM todo: MASS concentration or UNIT concentration datums</t>
+MAM done/check: MASS concentration or UNIT concentration datums</t>
         </r>
       </text>
     </comment>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -475,9 +475,6 @@
     <t>blood plasma specimen|blood serum specimen</t>
   </si>
   <si>
-    <t>concentration measurment datum</t>
-  </si>
-  <si>
     <t>glucose</t>
   </si>
   <si>
@@ -556,9 +553,6 @@
     <t>http://transformunify.org/ontologies/TURBO_0010732</t>
   </si>
   <si>
-    <t>volume per volume datum</t>
-  </si>
-  <si>
     <t>erythrocyte</t>
   </si>
   <si>
@@ -617,13 +611,28 @@
   </si>
   <si>
     <t>automated measuring count of neutrophils in blood</t>
+  </si>
+  <si>
+    <t>confirmatory assay</t>
+  </si>
+  <si>
+    <t>automated assay</t>
+  </si>
+  <si>
+    <t>mass/volume concentration datum</t>
+  </si>
+  <si>
+    <t>volume/volume percentage concentration datum</t>
+  </si>
+  <si>
+    <t>arbitrary units per 24 hours datum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,6 +784,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1122,9 +1137,10 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1450,7 +1466,7 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,10 +1493,10 @@
     <col min="20" max="20" width="85.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="17.28515625" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="88.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1552,7 +1568,7 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
@@ -1635,7 +1651,7 @@
       <c r="V2" t="s">
         <v>47</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="X2" t="s">
@@ -1659,10 +1675,10 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
         <v>55</v>
@@ -1673,25 +1689,25 @@
       <c r="Q3" t="s">
         <v>57</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA3" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L4" t="s">
         <v>55</v>
@@ -1700,27 +1716,27 @@
         <v>56</v>
       </c>
       <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="W4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L5" t="s">
         <v>55</v>
@@ -1729,27 +1745,27 @@
         <v>56</v>
       </c>
       <c r="Q5" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AA5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
         <v>55</v>
@@ -1758,27 +1774,27 @@
         <v>56</v>
       </c>
       <c r="Q6" t="s">
+        <v>67</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA6" t="s">
         <v>68</v>
       </c>
-      <c r="W6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="AB6" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
         <v>55</v>
@@ -1787,30 +1803,30 @@
         <v>56</v>
       </c>
       <c r="O7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB7" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>68</v>
-      </c>
-      <c r="W7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s">
         <v>55</v>
@@ -1818,28 +1834,31 @@
       <c r="N8" t="s">
         <v>56</v>
       </c>
+      <c r="P8" t="s">
+        <v>104</v>
+      </c>
       <c r="Q8" t="s">
-        <v>68</v>
-      </c>
-      <c r="W8" t="s">
-        <v>58</v>
+        <v>67</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AA8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB8" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L9" t="s">
         <v>55</v>
@@ -1850,25 +1869,25 @@
       <c r="Q9" t="s">
         <v>57</v>
       </c>
-      <c r="W9" t="s">
-        <v>58</v>
+      <c r="W9" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AA9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB9" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L10" t="s">
         <v>55</v>
@@ -1876,28 +1895,31 @@
       <c r="N10" t="s">
         <v>56</v>
       </c>
+      <c r="P10" t="s">
+        <v>105</v>
+      </c>
       <c r="Q10" t="s">
-        <v>62</v>
-      </c>
-      <c r="W10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA10" t="s">
         <v>81</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
         <v>55</v>
@@ -1905,17 +1927,20 @@
       <c r="N11" t="s">
         <v>56</v>
       </c>
+      <c r="P11" t="s">
+        <v>105</v>
+      </c>
       <c r="Q11" t="s">
-        <v>62</v>
-      </c>
-      <c r="W11" t="s">
+        <v>61</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB11" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1928,8 +1953,10 @@
     <hyperlink ref="AB9" r:id="rId6"/>
     <hyperlink ref="AB10" r:id="rId7"/>
     <hyperlink ref="AB11" r:id="rId8"/>
+    <hyperlink ref="AB3" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>